<commit_message>
Remove outdated evaluation files and update .gitignore to exclude .conda files
</commit_message>
<xml_diff>
--- a/eval_pb_note.xlsx
+++ b/eval_pb_note.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="Polaris Office Sheet" lastEdited="4" lowestEdited="4" rupBuild="10.105.269.55310"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="580" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" tabRatio="570" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$141</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
   <si>
     <t>dataset</t>
   </si>
@@ -624,6 +624,9 @@
   </si>
   <si>
     <t>singleop</t>
+  </si>
+  <si>
+    <t>winograd(commonsense)</t>
   </si>
 </sst>
 </file>
@@ -1636,14 +1639,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D141"/>
   <sheetViews>
-    <sheetView topLeftCell="A121" tabSelected="1" zoomScale="120" workbookViewId="0">
-      <selection activeCell="F139" sqref="F139"/>
+    <sheetView tabSelected="1" zoomScale="120" workbookViewId="0">
+      <selection activeCell="F145" sqref="F145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.500000"/>
   <cols>
-    <col min="1" max="1" width="12.25500011" customWidth="1" outlineLevel="0"/>
-    <col min="3" max="3" width="13.00500011" customWidth="1" outlineLevel="0"/>
+    <col min="1" max="1" width="23.12999916" customWidth="1" outlineLevel="0"/>
+    <col min="3" max="3" width="21.75499916" customWidth="1" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.250000">
@@ -1660,9 +1663,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="16.500000" hidden="1">
       <c r="A2" s="0" t="s">
-        <v>33</v>
+        <v>195</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>4</v>
@@ -1674,9 +1677,9 @@
         <v>0.876923076923076</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="16.500000" hidden="1">
       <c r="A3" s="0" t="s">
-        <v>33</v>
+        <v>195</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>4</v>
@@ -1688,9 +1691,9 @@
         <v>0.871794871794871</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" ht="16.500000" hidden="1">
       <c r="A4" s="0" t="s">
-        <v>33</v>
+        <v>195</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>4</v>
@@ -1702,9 +1705,9 @@
         <v>0.871794871794871</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" ht="16.500000" hidden="1">
       <c r="A5" s="0" t="s">
-        <v>33</v>
+        <v>195</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>4</v>
@@ -1716,9 +1719,9 @@
         <v>0.871794871794871</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" ht="16.500000" hidden="1">
       <c r="A6" s="0" t="s">
-        <v>33</v>
+        <v>195</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>4</v>
@@ -1730,9 +1733,9 @@
         <v>0.861538461538461</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" ht="16.500000" hidden="1">
       <c r="A7" s="0" t="s">
-        <v>33</v>
+        <v>195</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>4</v>
@@ -1744,9 +1747,9 @@
         <v>0.856410256410256</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" ht="16.500000" hidden="1">
       <c r="A8" s="0" t="s">
-        <v>33</v>
+        <v>195</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>4</v>
@@ -1758,9 +1761,9 @@
         <v>0.851282051282051</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" ht="16.500000" hidden="1">
       <c r="A9" s="0" t="s">
-        <v>33</v>
+        <v>195</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>4</v>
@@ -1772,9 +1775,9 @@
         <v>0.841025641025641</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" ht="16.500000" hidden="1">
       <c r="A10" s="0" t="s">
-        <v>33</v>
+        <v>195</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>4</v>
@@ -1786,9 +1789,9 @@
         <v>0.866666666666666</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" ht="16.500000" hidden="1">
       <c r="A11" s="0" t="s">
-        <v>33</v>
+        <v>195</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>4</v>
@@ -1800,9 +1803,9 @@
         <v>0.866666666666666</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" ht="16.500000" hidden="1">
       <c r="A12" s="0" t="s">
-        <v>33</v>
+        <v>195</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>4</v>
@@ -1814,9 +1817,9 @@
         <v>0.866666666666666</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" ht="16.500000" hidden="1">
       <c r="A13" s="0" t="s">
-        <v>33</v>
+        <v>195</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>4</v>
@@ -1828,9 +1831,9 @@
         <v>0.866666666666666</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" ht="16.500000" hidden="1">
       <c r="A14" s="0" t="s">
-        <v>33</v>
+        <v>195</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>4</v>
@@ -1842,9 +1845,9 @@
         <v>0.866666666666666</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" ht="16.500000" hidden="1">
       <c r="A15" s="0" t="s">
-        <v>33</v>
+        <v>195</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>4</v>
@@ -1856,7 +1859,7 @@
         <v>0.856410256410256</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" ht="16.500000" hidden="1">
       <c r="A16" s="0" t="s">
         <v>63</v>
       </c>
@@ -1870,7 +1873,7 @@
         <v>0.92822966507177</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" ht="16.500000" hidden="1">
       <c r="A17" s="0" t="s">
         <v>63</v>
       </c>
@@ -1884,7 +1887,7 @@
         <v>0.92822966507177</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" ht="16.500000" hidden="1">
       <c r="A18" s="0" t="s">
         <v>63</v>
       </c>
@@ -1898,7 +1901,7 @@
         <v>0.937799043062201</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" ht="16.500000" hidden="1">
       <c r="A19" s="0" t="s">
         <v>63</v>
       </c>
@@ -1912,7 +1915,7 @@
         <v>0.937799043062201</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" ht="16.500000" hidden="1">
       <c r="A20" s="0" t="s">
         <v>63</v>
       </c>
@@ -1926,7 +1929,7 @@
         <v>0.937799043062201</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" ht="16.500000" hidden="1">
       <c r="A21" s="0" t="s">
         <v>63</v>
       </c>
@@ -1940,7 +1943,7 @@
         <v>0.92822966507177</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" ht="16.500000" hidden="1">
       <c r="A22" s="0" t="s">
         <v>63</v>
       </c>
@@ -1954,7 +1957,7 @@
         <v>0.909090909090909</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" ht="16.500000" hidden="1">
       <c r="A23" s="0" t="s">
         <v>63</v>
       </c>
@@ -1968,7 +1971,7 @@
         <v>0.918660287081339</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" ht="16.500000" hidden="1">
       <c r="A24" s="0" t="s">
         <v>63</v>
       </c>
@@ -1982,7 +1985,7 @@
         <v>0.942583732057416</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" ht="16.500000" hidden="1">
       <c r="A25" s="0" t="s">
         <v>63</v>
       </c>
@@ -1996,7 +1999,7 @@
         <v>0.933014354066985</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" ht="16.500000" hidden="1">
       <c r="A26" s="0" t="s">
         <v>63</v>
       </c>
@@ -2010,7 +2013,7 @@
         <v>0.942583732057416</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" ht="16.500000" hidden="1">
       <c r="A27" s="0" t="s">
         <v>63</v>
       </c>
@@ -2024,7 +2027,7 @@
         <v>0.933014354066985</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" ht="16.500000" hidden="1">
       <c r="A28" s="0" t="s">
         <v>63</v>
       </c>
@@ -2038,7 +2041,7 @@
         <v>0.889952153110047</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" ht="16.500000" hidden="1">
       <c r="A29" s="0" t="s">
         <v>63</v>
       </c>
@@ -2052,7 +2055,7 @@
         <v>0.933014354066985</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" ht="16.500000" hidden="1">
       <c r="A30" s="0" t="s">
         <v>78</v>
       </c>
@@ -2060,13 +2063,13 @@
         <v>4</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D30" s="0">
-        <v>0.966789667896679</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>0.977859778597786</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="16.500000" hidden="1">
       <c r="A31" s="0" t="s">
         <v>78</v>
       </c>
@@ -2074,13 +2077,13 @@
         <v>4</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D31" s="0">
-        <v>0.970479704797047</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>0.974169741697417</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="16.500000" hidden="1">
       <c r="A32" s="0" t="s">
         <v>78</v>
       </c>
@@ -2088,13 +2091,13 @@
         <v>4</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D32" s="0">
-        <v>0.977859778597786</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>0.970479704797047</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="16.500000" hidden="1">
       <c r="A33" s="0" t="s">
         <v>78</v>
       </c>
@@ -2108,7 +2111,7 @@
         <v>0.959409594095941</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" ht="16.500000" hidden="1">
       <c r="A34" s="0" t="s">
         <v>78</v>
       </c>
@@ -2122,7 +2125,7 @@
         <v>0.966789667896679</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" ht="16.500000" hidden="1">
       <c r="A35" s="0" t="s">
         <v>78</v>
       </c>
@@ -2136,7 +2139,7 @@
         <v>0.974169741697417</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" ht="16.500000" hidden="1">
       <c r="A36" s="0" t="s">
         <v>78</v>
       </c>
@@ -2150,7 +2153,7 @@
         <v>0.966789667896679</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" ht="16.500000" hidden="1">
       <c r="A37" s="0" t="s">
         <v>78</v>
       </c>
@@ -2158,13 +2161,13 @@
         <v>4</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D37" s="0">
-        <v>0.966789667896679</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
+        <v>0.970479704797047</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="16.500000" hidden="1">
       <c r="A38" s="0" t="s">
         <v>78</v>
       </c>
@@ -2172,13 +2175,13 @@
         <v>4</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D38" s="0">
-        <v>0.974169741697417</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+        <v>0.966789667896679</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="16.500000" hidden="1">
       <c r="A39" s="0" t="s">
         <v>78</v>
       </c>
@@ -2192,7 +2195,7 @@
         <v>0.974169741697417</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" ht="16.500000" hidden="1">
       <c r="A40" s="0" t="s">
         <v>78</v>
       </c>
@@ -2206,7 +2209,7 @@
         <v>0.977859778597786</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" ht="16.500000" hidden="1">
       <c r="A41" s="0" t="s">
         <v>78</v>
       </c>
@@ -2220,7 +2223,7 @@
         <v>0.977859778597786</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" ht="16.500000" hidden="1">
       <c r="A42" s="0" t="s">
         <v>78</v>
       </c>
@@ -2234,7 +2237,7 @@
         <v>0.974169741697417</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" ht="16.500000" hidden="1">
       <c r="A43" s="0" t="s">
         <v>78</v>
       </c>
@@ -2242,13 +2245,13 @@
         <v>4</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D43" s="0">
-        <v>0.970479704797047</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
+        <v>0.966789667896679</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="16.500000" hidden="1">
       <c r="A44" s="0" t="s">
         <v>93</v>
       </c>
@@ -2256,13 +2259,13 @@
         <v>4</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D44" s="0">
-        <v>0.944751381215469</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+        <v>0.955801104972375</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="16.500000" hidden="1">
       <c r="A45" s="0" t="s">
         <v>93</v>
       </c>
@@ -2270,13 +2273,13 @@
         <v>4</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D45" s="0">
-        <v>0.955801104972375</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
+        <v>0.944751381215469</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="16.500000" hidden="1">
       <c r="A46" s="0" t="s">
         <v>93</v>
       </c>
@@ -2284,13 +2287,13 @@
         <v>4</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D46" s="0">
-        <v>0.939226519337016</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
+        <v>0.944751381215469</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="16.500000" hidden="1">
       <c r="A47" s="0" t="s">
         <v>93</v>
       </c>
@@ -2304,7 +2307,7 @@
         <v>0.944751381215469</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" ht="16.500000" hidden="1">
       <c r="A48" s="0" t="s">
         <v>93</v>
       </c>
@@ -2318,7 +2321,7 @@
         <v>0.922651933701657</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" ht="16.500000" hidden="1">
       <c r="A49" s="0" t="s">
         <v>93</v>
       </c>
@@ -2332,7 +2335,7 @@
         <v>0.939226519337016</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" ht="16.500000" hidden="1">
       <c r="A50" s="0" t="s">
         <v>93</v>
       </c>
@@ -2346,7 +2349,7 @@
         <v>0.950276243093922</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" ht="16.500000" hidden="1">
       <c r="A51" s="0" t="s">
         <v>93</v>
       </c>
@@ -2354,13 +2357,13 @@
         <v>4</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D51" s="0">
         <v>0.944751381215469</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" ht="16.500000" hidden="1">
       <c r="A52" s="0" t="s">
         <v>93</v>
       </c>
@@ -2368,13 +2371,13 @@
         <v>4</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D52" s="0">
-        <v>0.944751381215469</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+        <v>0.939226519337016</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="16.500000" hidden="1">
       <c r="A53" s="0" t="s">
         <v>93</v>
       </c>
@@ -2388,7 +2391,7 @@
         <v>0.944751381215469</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" ht="16.500000" hidden="1">
       <c r="A54" s="0" t="s">
         <v>93</v>
       </c>
@@ -2402,7 +2405,7 @@
         <v>0.944751381215469</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" ht="16.500000" hidden="1">
       <c r="A55" s="0" t="s">
         <v>93</v>
       </c>
@@ -2416,7 +2419,7 @@
         <v>0.944751381215469</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" ht="16.500000" hidden="1">
       <c r="A56" s="0" t="s">
         <v>93</v>
       </c>
@@ -2430,7 +2433,7 @@
         <v>0.950276243093922</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" ht="16.500000" hidden="1">
       <c r="A57" s="0" t="s">
         <v>93</v>
       </c>
@@ -2444,7 +2447,7 @@
         <v>0.933701657458563</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" ht="16.500000" hidden="1">
       <c r="A58" s="0" t="s">
         <v>108</v>
       </c>
@@ -2452,13 +2455,13 @@
         <v>4</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D58" s="0">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="16.500000" hidden="1">
       <c r="A59" s="0" t="s">
         <v>108</v>
       </c>
@@ -2466,13 +2469,13 @@
         <v>4</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D59" s="0">
         <v>0.99</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" ht="16.500000" hidden="1">
       <c r="A60" s="0" t="s">
         <v>108</v>
       </c>
@@ -2480,13 +2483,13 @@
         <v>4</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D60" s="0">
-        <v>0.995</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="16.500000" hidden="1">
       <c r="A61" s="0" t="s">
         <v>108</v>
       </c>
@@ -2500,7 +2503,7 @@
         <v>0.985</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" ht="16.500000" hidden="1">
       <c r="A62" s="0" t="s">
         <v>108</v>
       </c>
@@ -2514,7 +2517,7 @@
         <v>0.995</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" ht="16.500000" hidden="1">
       <c r="A63" s="0" t="s">
         <v>108</v>
       </c>
@@ -2528,7 +2531,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" ht="16.500000" hidden="1">
       <c r="A64" s="0" t="s">
         <v>108</v>
       </c>
@@ -2542,7 +2545,7 @@
         <v>0.995</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" ht="16.500000" hidden="1">
       <c r="A65" s="0" t="s">
         <v>108</v>
       </c>
@@ -2556,7 +2559,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" ht="16.500000" hidden="1">
       <c r="A66" s="0" t="s">
         <v>108</v>
       </c>
@@ -2570,7 +2573,7 @@
         <v>0.985</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" ht="16.500000" hidden="1">
       <c r="A67" s="0" t="s">
         <v>108</v>
       </c>
@@ -2584,7 +2587,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" ht="16.500000" hidden="1">
       <c r="A68" s="0" t="s">
         <v>108</v>
       </c>
@@ -2598,7 +2601,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" ht="16.500000" hidden="1">
       <c r="A69" s="0" t="s">
         <v>108</v>
       </c>
@@ -2612,7 +2615,7 @@
         <v>0.985</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" ht="16.500000" hidden="1">
       <c r="A70" s="0" t="s">
         <v>108</v>
       </c>
@@ -2626,7 +2629,7 @@
         <v>0.995</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" ht="16.500000" hidden="1">
       <c r="A71" s="0" t="s">
         <v>108</v>
       </c>
@@ -2640,7 +2643,7 @@
         <v>0.985</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" ht="16.500000" hidden="1">
       <c r="A72" s="0" t="s">
         <v>123</v>
       </c>
@@ -2654,7 +2657,7 @@
         <v>0.898876404494382</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" ht="16.500000" hidden="1">
       <c r="A73" s="0" t="s">
         <v>123</v>
       </c>
@@ -2668,7 +2671,7 @@
         <v>0.906367041198501</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" ht="16.500000" hidden="1">
       <c r="A74" s="0" t="s">
         <v>123</v>
       </c>
@@ -2682,7 +2685,7 @@
         <v>0.895131086142322</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" ht="16.500000" hidden="1">
       <c r="A75" s="0" t="s">
         <v>123</v>
       </c>
@@ -2696,7 +2699,7 @@
         <v>0.895131086142322</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" ht="16.500000" hidden="1">
       <c r="A76" s="0" t="s">
         <v>123</v>
       </c>
@@ -2710,7 +2713,7 @@
         <v>0.895131086142322</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" ht="16.500000" hidden="1">
       <c r="A77" s="0" t="s">
         <v>123</v>
       </c>
@@ -2724,7 +2727,7 @@
         <v>0.891385767790262</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" ht="16.500000" hidden="1">
       <c r="A78" s="0" t="s">
         <v>123</v>
       </c>
@@ -2738,7 +2741,7 @@
         <v>0.891385767790262</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" ht="16.500000" hidden="1">
       <c r="A79" s="0" t="s">
         <v>123</v>
       </c>
@@ -2752,7 +2755,7 @@
         <v>0.895131086142322</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" ht="16.500000" hidden="1">
       <c r="A80" s="0" t="s">
         <v>123</v>
       </c>
@@ -2766,7 +2769,7 @@
         <v>0.902621722846441</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" ht="16.500000" hidden="1">
       <c r="A81" s="0" t="s">
         <v>123</v>
       </c>
@@ -2780,7 +2783,7 @@
         <v>0.898876404494382</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" ht="16.500000" hidden="1">
       <c r="A82" s="0" t="s">
         <v>123</v>
       </c>
@@ -2794,7 +2797,7 @@
         <v>0.910112359550561</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" ht="16.500000" hidden="1">
       <c r="A83" s="0" t="s">
         <v>123</v>
       </c>
@@ -2808,7 +2811,7 @@
         <v>0.913857677902621</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" ht="16.500000" hidden="1">
       <c r="A84" s="0" t="s">
         <v>123</v>
       </c>
@@ -2822,7 +2825,7 @@
         <v>0.872659176029962</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" ht="16.500000" hidden="1">
       <c r="A85" s="0" t="s">
         <v>123</v>
       </c>
@@ -2836,7 +2839,7 @@
         <v>0.910112359550561</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" ht="16.500000" hidden="1">
       <c r="A86" s="0" t="s">
         <v>138</v>
       </c>
@@ -2850,7 +2853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" ht="16.500000" hidden="1">
       <c r="A87" s="0" t="s">
         <v>138</v>
       </c>
@@ -2864,7 +2867,7 @@
         <v>0.994117647058823</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" ht="16.500000" hidden="1">
       <c r="A88" s="0" t="s">
         <v>138</v>
       </c>
@@ -2878,7 +2881,7 @@
         <v>0.994117647058823</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" ht="16.500000" hidden="1">
       <c r="A89" s="0" t="s">
         <v>138</v>
       </c>
@@ -2892,7 +2895,7 @@
         <v>0.994117647058823</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" ht="16.500000" hidden="1">
       <c r="A90" s="0" t="s">
         <v>138</v>
       </c>
@@ -2906,7 +2909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" ht="16.500000" hidden="1">
       <c r="A91" s="0" t="s">
         <v>138</v>
       </c>
@@ -2920,7 +2923,7 @@
         <v>0.988235294117647</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" ht="16.500000" hidden="1">
       <c r="A92" s="0" t="s">
         <v>138</v>
       </c>
@@ -2934,7 +2937,7 @@
         <v>0.994117647058823</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" ht="16.500000" hidden="1">
       <c r="A93" s="0" t="s">
         <v>138</v>
       </c>
@@ -2948,7 +2951,7 @@
         <v>0.994117647058823</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" ht="16.500000" hidden="1">
       <c r="A94" s="0" t="s">
         <v>138</v>
       </c>
@@ -2962,7 +2965,7 @@
         <v>0.994117647058823</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:4" ht="16.500000" hidden="1">
       <c r="A95" s="0" t="s">
         <v>138</v>
       </c>
@@ -2976,7 +2979,7 @@
         <v>0.988235294117647</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" ht="16.500000" hidden="1">
       <c r="A96" s="0" t="s">
         <v>138</v>
       </c>
@@ -2990,7 +2993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" ht="16.500000" hidden="1">
       <c r="A97" s="0" t="s">
         <v>138</v>
       </c>
@@ -3004,7 +3007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" ht="16.500000" hidden="1">
       <c r="A98" s="0" t="s">
         <v>138</v>
       </c>
@@ -3018,7 +3021,7 @@
         <v>0.994117647058823</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" ht="16.500000" hidden="1">
       <c r="A99" s="0" t="s">
         <v>138</v>
       </c>
@@ -3032,7 +3035,7 @@
         <v>0.994117647058823</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" ht="16.500000" hidden="1">
       <c r="A100" s="0" t="s">
         <v>154</v>
       </c>
@@ -3046,7 +3049,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" ht="16.500000" hidden="1">
       <c r="A101" s="0" t="s">
         <v>154</v>
       </c>
@@ -3054,13 +3057,13 @@
         <v>4</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D101" s="0">
-        <v>0.965</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="16.500000" hidden="1">
       <c r="A102" s="0" t="s">
         <v>154</v>
       </c>
@@ -3068,13 +3071,13 @@
         <v>4</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D102" s="0">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4">
+        <v>0.965</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="16.500000" hidden="1">
       <c r="A103" s="0" t="s">
         <v>154</v>
       </c>
@@ -3088,7 +3091,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" ht="16.500000" hidden="1">
       <c r="A104" s="0" t="s">
         <v>154</v>
       </c>
@@ -3102,7 +3105,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" ht="16.500000" hidden="1">
       <c r="A105" s="0" t="s">
         <v>154</v>
       </c>
@@ -3116,7 +3119,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" ht="16.500000" hidden="1">
       <c r="A106" s="0" t="s">
         <v>154</v>
       </c>
@@ -3130,7 +3133,7 @@
         <v>0.915</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" ht="16.500000" hidden="1">
       <c r="A107" s="0" t="s">
         <v>154</v>
       </c>
@@ -3144,7 +3147,7 @@
         <v>0.965</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" ht="16.500000" hidden="1">
       <c r="A108" s="0" t="s">
         <v>154</v>
       </c>
@@ -3158,7 +3161,7 @@
         <v>0.965</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" ht="16.500000" hidden="1">
       <c r="A109" s="0" t="s">
         <v>154</v>
       </c>
@@ -3172,7 +3175,7 @@
         <v>0.975</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:4" ht="16.500000" hidden="1">
       <c r="A110" s="0" t="s">
         <v>154</v>
       </c>
@@ -3186,7 +3189,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" ht="16.500000" hidden="1">
       <c r="A111" s="0" t="s">
         <v>154</v>
       </c>
@@ -3200,7 +3203,7 @@
         <v>0.965</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:4" ht="16.500000" hidden="1">
       <c r="A112" s="0" t="s">
         <v>154</v>
       </c>
@@ -3214,7 +3217,7 @@
         <v>0.92</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:4" ht="16.500000" hidden="1">
       <c r="A113" s="0" t="s">
         <v>154</v>
       </c>
@@ -3236,10 +3239,10 @@
         <v>4</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D114" s="0">
-        <v>0.931578947368421</v>
+        <v>0.942105263157894</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -3250,10 +3253,10 @@
         <v>4</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="D115" s="0">
-        <v>0.931578947368421</v>
+        <v>0.936842105263157</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -3264,13 +3267,13 @@
         <v>4</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D116" s="0">
-        <v>0.926315789473684</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4">
+        <v>0.931578947368421</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="16.500000" hidden="1">
       <c r="A117" s="0" t="s">
         <v>179</v>
       </c>
@@ -3284,7 +3287,7 @@
         <v>0.931578947368421</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:4" ht="16.500000" hidden="1">
       <c r="A118" s="0" t="s">
         <v>179</v>
       </c>
@@ -3298,7 +3301,7 @@
         <v>0.91578947368421</v>
       </c>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:4" ht="16.500000" hidden="1">
       <c r="A119" s="0" t="s">
         <v>179</v>
       </c>
@@ -3312,7 +3315,7 @@
         <v>0.931578947368421</v>
       </c>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:4" ht="16.500000" hidden="1">
       <c r="A120" s="0" t="s">
         <v>179</v>
       </c>
@@ -3334,10 +3337,10 @@
         <v>4</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D121" s="0">
-        <v>0.942105263157894</v>
+        <v>0.931578947368421</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -3348,13 +3351,13 @@
         <v>4</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D122" s="0">
         <v>0.926315789473684</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:4" ht="16.500000" hidden="1">
       <c r="A123" s="0" t="s">
         <v>179</v>
       </c>
@@ -3368,7 +3371,7 @@
         <v>0.936842105263157</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:4" ht="16.500000" hidden="1">
       <c r="A124" s="0" t="s">
         <v>179</v>
       </c>
@@ -3382,7 +3385,7 @@
         <v>0.942105263157894</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:4" ht="16.500000" hidden="1">
       <c r="A125" s="0" t="s">
         <v>179</v>
       </c>
@@ -3396,7 +3399,7 @@
         <v>0.936842105263157</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:4" ht="16.500000" hidden="1">
       <c r="A126" s="0" t="s">
         <v>179</v>
       </c>
@@ -3418,13 +3421,13 @@
         <v>4</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D127" s="0">
-        <v>0.936842105263157</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4">
+        <v>0.926315789473684</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="16.500000" hidden="1">
       <c r="A128" s="0" t="s">
         <v>194</v>
       </c>
@@ -3438,7 +3441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="2:3">
+    <row r="129" spans="1:4" ht="16.500000" hidden="1">
       <c r="A129" s="0" t="s">
         <v>194</v>
       </c>
@@ -3452,7 +3455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="2:3">
+    <row r="130" spans="1:4" ht="16.500000" hidden="1">
       <c r="A130" s="0" t="s">
         <v>194</v>
       </c>
@@ -3466,7 +3469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="2:3">
+    <row r="131" spans="1:4" ht="16.500000" hidden="1">
       <c r="A131" s="0" t="s">
         <v>194</v>
       </c>
@@ -3480,7 +3483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="2:3">
+    <row r="132" spans="1:4" ht="16.500000" hidden="1">
       <c r="A132" s="0" t="s">
         <v>194</v>
       </c>
@@ -3494,7 +3497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="2:3">
+    <row r="133" spans="1:4" ht="16.500000" hidden="1">
       <c r="A133" s="0" t="s">
         <v>194</v>
       </c>
@@ -3508,7 +3511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="2:3">
+    <row r="134" spans="1:4" ht="16.500000" hidden="1">
       <c r="A134" s="0" t="s">
         <v>194</v>
       </c>
@@ -3522,7 +3525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="2:3">
+    <row r="135" spans="1:4" ht="16.500000" hidden="1">
       <c r="A135" s="0" t="s">
         <v>194</v>
       </c>
@@ -3536,7 +3539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="2:3">
+    <row r="136" spans="1:4" ht="16.500000" hidden="1">
       <c r="A136" s="0" t="s">
         <v>194</v>
       </c>
@@ -3550,7 +3553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="2:3">
+    <row r="137" spans="1:4" ht="16.500000" hidden="1">
       <c r="A137" s="0" t="s">
         <v>194</v>
       </c>
@@ -3564,7 +3567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="2:3">
+    <row r="138" spans="1:4" ht="16.500000" hidden="1">
       <c r="A138" s="0" t="s">
         <v>194</v>
       </c>
@@ -3578,7 +3581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="2:3">
+    <row r="139" spans="1:4" ht="16.500000" hidden="1">
       <c r="A139" s="0" t="s">
         <v>194</v>
       </c>
@@ -3592,7 +3595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="2:3">
+    <row r="140" spans="1:4" ht="16.500000" hidden="1">
       <c r="A140" s="0" t="s">
         <v>194</v>
       </c>
@@ -3606,7 +3609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="2:3">
+    <row r="141" spans="1:4" ht="16.500000" hidden="1">
       <c r="A141" s="0" t="s">
         <v>194</v>
       </c>
@@ -3621,9 +3624,24 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D15">
+  <autoFilter ref="A1:D141">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="object"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="platinum_prompt"/>
+        <filter val="platinum_prompt_no_cot"/>
+        <filter val="RE2"/>
+        <filter val="RE2_no_cot"/>
+        <filter val="sRE2"/>
+        <filter val="sRE2_no_cot"/>
+      </filters>
+    </filterColumn>
     <sortState ref="A2:D141">
-      <sortCondition descending="1" ref="D2:D15"/>
+      <sortCondition descending="1" ref="D2:D141"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>